<commit_message>
added non - carry over option
</commit_message>
<xml_diff>
--- a/v2-Implementation/Data/Data-complex-newcost.xlsx
+++ b/v2-Implementation/Data/Data-complex-newcost.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Indices Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="44">
   <si>
     <t>Time Horizon (t)</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Cost of Rescheduling Premium (cc)</t>
+  </si>
+  <si>
+    <t>-5,5</t>
   </si>
 </sst>
 </file>
@@ -369,7 +372,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-CA"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -785,11 +788,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="100941120"/>
-        <c:axId val="290365440"/>
+        <c:axId val="183826624"/>
+        <c:axId val="183827200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100941120"/>
+        <c:axId val="183826624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -799,12 +802,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="290365440"/>
+        <c:crossAx val="183827200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="290365440"/>
+        <c:axId val="183827200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -815,14 +818,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100941120"/>
+        <c:crossAx val="183826624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1329,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,7 +1368,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1374,7 +1376,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="3">
         <v>20</v>
@@ -2329,9 +2331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
finished changing complexity transitions
</commit_message>
<xml_diff>
--- a/v2-Implementation/Data/Data-complex-newcost.xlsx
+++ b/v2-Implementation/Data/Data-complex-newcost.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Indices Data" sheetId="1" r:id="rId1"/>
@@ -341,6 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -348,7 +349,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -373,7 +373,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-CA"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -789,11 +789,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="185923200"/>
-        <c:axId val="185923776"/>
+        <c:axId val="101137728"/>
+        <c:axId val="217817088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="185923200"/>
+        <c:axId val="101137728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,12 +803,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185923776"/>
+        <c:crossAx val="217817088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="185923776"/>
+        <c:axId val="217817088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -819,7 +819,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="185923200"/>
+        <c:crossAx val="101137728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1668,7 +1668,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1692,7 +1694,7 @@
       <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="33"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -2470,7 +2472,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2794,23 +2798,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="30" t="s">
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
     </row>
     <row r="2" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -7050,7 +7054,7 @@
   <dimension ref="A1:R442"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7075,34 +7079,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="31" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="30" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="30" t="s">
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="31" t="s">
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
     </row>
     <row r="2" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">

</xml_diff>